<commit_message>
Fix bugs and add tests
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_5.xlsx
+++ b/tests/integration_test_files/full_5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E601C5CC-079E-4945-B4D5-393D4508D49C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D73C8D-9578-6340-9C38-012C3E5A926C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30120" yWindow="500" windowWidth="58640" windowHeight="23700" firstSheet="7" activeTab="24" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
@@ -2838,10 +2838,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8136,120 +8136,120 @@
       <c r="A1" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="51" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
     </row>
     <row r="3" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="52" t="s">
         <v>806</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
     </row>
     <row r="4" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="51" t="s">
         <v>129</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
       <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
       <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="52" t="s">
         <v>678</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
       <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="52" t="s">
         <v>707</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
       <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -8341,16 +8341,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11984,6 +11984,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D47D794EB48E7144959FE534A5ED3D9A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2a26abefe6b107b571df4f2e43af2ce">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98eacbea-7562-4a40-a7f2-e999cdc0cec5" xmlns:ns3="75bf9804-c18d-470a-a27f-eeaf4abcd247" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5806404ce956f9af473b927dc8d5ee33" ns2:_="" ns3:_="">
     <xsd:import namespace="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
@@ -12184,15 +12193,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
   <ds:schemaRefs>
@@ -12211,6 +12211,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028E3775-7751-44E5-835D-F091B807F690}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12227,12 +12235,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>